<commit_message>
Patching code to run pba.py v0.14
</commit_message>
<xml_diff>
--- a/CO2_carbonfootprint_model_FBDO_DSS.xlsx
+++ b/CO2_carbonfootprint_model_FBDO_DSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Francis/PycharmProjects/VerticalFarming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F10AD061-4110-8B40-992F-9612910D6F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA7FC72-7F74-AA40-9A01-C24443366F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33420" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="572">
   <si>
     <t>Sources:</t>
   </si>
@@ -2780,7 +2780,6 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2800,6 +2799,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2835,7 +2835,9 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -12115,15 +12117,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12146,7 +12148,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22339300" y="11391900"/>
+          <a:off x="25019000" y="9232900"/>
           <a:ext cx="7442200" cy="4051300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12374,7 +12376,7 @@
   <dimension ref="A1:O1030"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D203" sqref="D203"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -13524,7 +13526,7 @@
       <c r="D92" s="103" t="s">
         <v>469</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="56" t="s">
         <v>470</v>
       </c>
     </row>
@@ -15782,10 +15784,11 @@
     <hyperlink ref="M137" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="M176" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="M114" r:id="rId8" xr:uid="{CBD5C97D-B061-C34B-91EF-E7D5CF4C5EDB}"/>
+    <hyperlink ref="F92" r:id="rId9" xr:uid="{9160B818-CEA2-A54C-8E92-CD1FF52040C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -15821,180 +15824,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="153" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="154" t="s">
         <v>520</v>
       </c>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="155" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="154" t="s">
         <v>521</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="154" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="155" t="s">
+      <c r="C4" s="154" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="155" t="s">
+      <c r="A5" s="154" t="s">
         <v>523</v>
       </c>
-      <c r="B5" s="157">
+      <c r="B5" s="156">
         <v>159</v>
       </c>
-      <c r="C5" s="155" t="s">
+      <c r="C5" s="154" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="154" t="s">
         <v>524</v>
       </c>
-      <c r="B6" s="157">
+      <c r="B6" s="156">
         <v>1330</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="154" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="155" t="s">
+      <c r="A7" s="154" t="s">
         <v>525</v>
       </c>
-      <c r="B7" s="155">
+      <c r="B7" s="154">
         <f>SUM(B5:B6)</f>
         <v>1489</v>
       </c>
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="154" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="155" t="s">
+      <c r="A8" s="154" t="s">
         <v>526</v>
       </c>
-      <c r="B8" s="155">
+      <c r="B8" s="154">
         <v>0.30399999999999999</v>
       </c>
-      <c r="C8" s="155" t="s">
+      <c r="C8" s="154" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="154" t="s">
         <v>528</v>
       </c>
-      <c r="B9" s="155">
+      <c r="B9" s="154">
         <f>89.4 + 3.23</f>
         <v>92.63000000000001</v>
       </c>
-      <c r="C9" s="157" t="s">
+      <c r="C9" s="156" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="155" t="s">
+      <c r="A11" s="154" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="155" t="s">
+      <c r="A12" s="154" t="s">
         <v>531</v>
       </c>
-      <c r="B12" s="155">
+      <c r="B12" s="154">
         <f>(60+80)/2</f>
         <v>70</v>
       </c>
-      <c r="C12" s="155" t="s">
+      <c r="C12" s="154" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="157" t="s">
         <v>533</v>
       </c>
-      <c r="B15" s="159">
+      <c r="B15" s="158">
         <f>ROUNDDOWN(B7/B12,2)</f>
         <v>21.27</v>
       </c>
-      <c r="C15" s="160" t="s">
+      <c r="C15" s="159" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="157" t="s">
         <v>534</v>
       </c>
-      <c r="B16" s="159">
+      <c r="B16" s="158">
         <f>ROUNDDOWN(B9/B12,2)</f>
         <v>1.32</v>
       </c>
-      <c r="C16" s="160" t="s">
+      <c r="C16" s="159" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="155" t="s">
+      <c r="A18" s="154" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="154" t="s">
         <v>536</v>
       </c>
-      <c r="B19" s="155">
+      <c r="B19" s="154">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="154" t="s">
         <v>537</v>
       </c>
-      <c r="B20" s="155">
+      <c r="B20" s="154">
         <v>64</v>
       </c>
-      <c r="C20" s="155" t="s">
+      <c r="C20" s="154" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="161" t="s">
+      <c r="A21" s="160" t="s">
         <v>539</v>
       </c>
-      <c r="B21" s="162">
+      <c r="B21" s="161">
         <f>B20/B19</f>
         <v>1.28</v>
       </c>
-      <c r="C21" s="162" t="s">
+      <c r="C21" s="161" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="155" t="s">
+      <c r="A23" s="154" t="s">
         <v>540</v>
       </c>
-      <c r="B23" s="155">
+      <c r="B23" s="154">
         <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="158" t="s">
+      <c r="A24" s="157" t="s">
         <v>541</v>
       </c>
-      <c r="B24" s="159">
+      <c r="B24" s="158">
         <f>(B21/1000)*B23*B16</f>
         <v>0.21626880000000004</v>
       </c>
-      <c r="C24" s="160" t="s">
+      <c r="C24" s="159" t="s">
         <v>529</v>
       </c>
     </row>
@@ -16011,7 +16014,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -16052,7 +16055,7 @@
       <c r="D4" t="s">
         <v>116</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="56" t="s">
         <v>117</v>
       </c>
     </row>
@@ -16066,7 +16069,7 @@
       <c r="C5" t="s">
         <v>119</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="56" t="s">
         <v>120</v>
       </c>
     </row>
@@ -17171,6 +17174,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="L5" r:id="rId2" xr:uid="{6A3DBCFD-688F-F44D-AFB6-F7D6EA820566}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17181,14 +17185,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="69.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="14" width="8.83203125" customWidth="1"/>
@@ -17952,7 +17956,7 @@
       <c r="D57" s="80" t="s">
         <v>285</v>
       </c>
-      <c r="E57" s="166" t="s">
+      <c r="E57" s="165" t="s">
         <v>275</v>
       </c>
       <c r="F57" s="80" t="s">
@@ -18060,41 +18064,41 @@
       <c r="B59" s="60" t="s">
         <v>271</v>
       </c>
-      <c r="C59" s="166" t="s">
+      <c r="C59" s="165" t="s">
         <v>280</v>
       </c>
-      <c r="D59" s="166" t="s">
+      <c r="D59" s="165" t="s">
         <v>284</v>
       </c>
       <c r="E59" s="60"/>
-      <c r="F59" s="166" t="s">
+      <c r="F59" s="165" t="s">
         <v>281</v>
       </c>
-      <c r="G59" s="166" t="s">
+      <c r="G59" s="165" t="s">
         <v>286</v>
       </c>
-      <c r="H59" s="166" t="s">
+      <c r="H59" s="165" t="s">
         <v>298</v>
       </c>
-      <c r="I59" s="167" t="s">
+      <c r="I59" s="166" t="s">
         <v>299</v>
       </c>
-      <c r="J59" s="166" t="s">
+      <c r="J59" s="165" t="s">
         <v>303</v>
       </c>
-      <c r="K59" s="166" t="s">
+      <c r="K59" s="165" t="s">
         <v>302</v>
       </c>
-      <c r="L59" s="167" t="s">
+      <c r="L59" s="166" t="s">
         <v>299</v>
       </c>
-      <c r="M59" s="166" t="s">
+      <c r="M59" s="165" t="s">
         <v>305</v>
       </c>
-      <c r="N59" s="166" t="s">
+      <c r="N59" s="165" t="s">
         <v>306</v>
       </c>
-      <c r="O59" s="166" t="s">
+      <c r="O59" s="165" t="s">
         <v>298</v>
       </c>
       <c r="P59" s="107" t="s">
@@ -18104,7 +18108,7 @@
       <c r="R59" s="107" t="s">
         <v>298</v>
       </c>
-      <c r="S59" s="166" t="s">
+      <c r="S59" s="165" t="s">
         <v>307</v>
       </c>
       <c r="T59" s="60"/>
@@ -18307,7 +18311,7 @@
       <c r="H64" s="80">
         <v>-112.5</v>
       </c>
-      <c r="I64" s="151" t="s">
+      <c r="I64" s="184" t="s">
         <v>552</v>
       </c>
       <c r="J64" s="80">
@@ -22091,8 +22095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2CCDBF-7B47-2448-A70D-0D37EF0474CE}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22243,7 +22247,7 @@
       </c>
       <c r="K5" s="125"/>
       <c r="L5" s="125"/>
-      <c r="M5" s="184">
+      <c r="M5" s="170">
         <f>Overview!B87</f>
         <v>2400</v>
       </c>
@@ -22290,7 +22294,7 @@
         <f>Overview!B121</f>
         <v>403.65000000000003</v>
       </c>
-      <c r="I6" s="164">
+      <c r="I6" s="163">
         <f>Overview!B41</f>
         <v>216</v>
       </c>
@@ -22308,7 +22312,7 @@
       <c r="O6" s="125">
         <v>0</v>
       </c>
-      <c r="P6" s="165">
+      <c r="P6" s="164">
         <f>'Carbon Footprint Life Cycle'!P5*Overview!B73</f>
         <v>17940</v>
       </c>
@@ -22344,7 +22348,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="169">
+      <c r="G7" s="168">
         <f>G6/$C$5</f>
         <v>8.5999999999999993E-2</v>
       </c>
@@ -22525,7 +22529,7 @@
       <c r="L12" s="124">
         <v>0</v>
       </c>
-      <c r="M12" s="153">
+      <c r="M12" s="152">
         <f>Overview!B88</f>
         <v>25</v>
       </c>
@@ -22627,7 +22631,7 @@
         <f>F13/C12</f>
         <v>1.5644444444444447E-2</v>
       </c>
-      <c r="G14" s="170">
+      <c r="G14" s="169">
         <f>G13/C12</f>
         <v>6.8800000000000007E-3</v>
       </c>
@@ -22722,8 +22726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1D95C7-F652-E842-8F87-8DA79347D561}">
   <dimension ref="A1:T128"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="J166" sqref="J166"/>
+    <sheetView topLeftCell="A95" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25990,7 +25994,7 @@
       <c r="K97" s="124">
         <v>0</v>
       </c>
-      <c r="L97" s="152">
+      <c r="L97" s="151">
         <f>L96*'Energy Consumption'!I64/1000</f>
         <v>203.07536229946518</v>
       </c>
@@ -26058,7 +26062,7 @@
         <f>K97/C97</f>
         <v>0</v>
       </c>
-      <c r="L98" s="168">
+      <c r="L98" s="167">
         <f>L97/C97</f>
         <v>1.3189826318458413</v>
       </c>
@@ -26299,7 +26303,7 @@
       <c r="K107" s="124">
         <v>0</v>
       </c>
-      <c r="L107" s="153">
+      <c r="L107" s="152">
         <f>L106*'Energy Consumption'!D64/1000</f>
         <v>1044.3875775401068</v>
       </c>
@@ -26608,7 +26612,7 @@
       <c r="K117" s="124">
         <v>0</v>
       </c>
-      <c r="L117" s="153">
+      <c r="L117" s="152">
         <f>L116*'Energy Consumption'!S64/1000</f>
         <v>116.04306417112296</v>
       </c>
@@ -26882,6 +26886,36 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="D104:H104"/>
+    <mergeCell ref="I104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="D114:H114"/>
+    <mergeCell ref="D94:H94"/>
+    <mergeCell ref="I94:L94"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="I84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="D74:H74"/>
+    <mergeCell ref="I74:L74"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="D54:H54"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="D64:H64"/>
+    <mergeCell ref="I64:L64"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="Q3:R3"/>
@@ -26895,36 +26929,6 @@
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="D74:H74"/>
-    <mergeCell ref="I74:L74"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="D54:H54"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="D64:H64"/>
-    <mergeCell ref="I64:L64"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D94:H94"/>
-    <mergeCell ref="I94:L94"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="I84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="D104:H104"/>
-    <mergeCell ref="I104:L104"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="D114:H114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -26937,7 +26941,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -27296,7 +27300,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -30932,7 +30936,7 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -31146,35 +31150,18 @@
     <row r="26" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="128" t="s">
-        <v>478</v>
-      </c>
-      <c r="B28" s="148">
-        <f>B21*B17/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>472</v>
-      </c>
+      <c r="A28" s="128"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="128" t="s">
-        <v>479</v>
-      </c>
-      <c r="B29" s="147">
-        <f>B28*0.75</f>
-        <v>0</v>
-      </c>
+      <c r="A29" s="128"/>
+      <c r="B29" s="147"/>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" s="128" t="s">
-        <v>480</v>
-      </c>
-      <c r="B30" s="147">
-        <f>B28+B29</f>
-        <v>0</v>
-      </c>
+      <c r="A30" s="128"/>
+      <c r="B30" s="147"/>
       <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1"/>
@@ -32170,7 +32157,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32179,152 +32166,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="154" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="153" t="s">
         <v>495</v>
       </c>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="155" t="s">
         <v>496</v>
       </c>
-      <c r="D2" s="155"/>
+      <c r="D2" s="154"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="154" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="154" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="155" t="s">
+      <c r="A5" s="154" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="154" t="s">
         <v>500</v>
       </c>
-      <c r="B6" s="155">
+      <c r="B6" s="154">
         <v>432</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="154" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="155"/>
-      <c r="B7" s="155">
+      <c r="A7" s="154"/>
+      <c r="B7" s="154">
         <v>45.1</v>
       </c>
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="154" t="s">
         <v>502</v>
       </c>
-      <c r="D7" s="155" t="s">
+      <c r="D7" s="154" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="157" t="s">
         <v>503</v>
       </c>
-      <c r="B8" s="159">
+      <c r="B8" s="158">
         <f>B6/300</f>
         <v>1.44</v>
       </c>
-      <c r="C8" s="159" t="s">
+      <c r="C8" s="158" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="155"/>
+      <c r="A9" s="154"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="154" t="s">
+      <c r="A10" s="153" t="s">
         <v>504</v>
       </c>
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="155" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="162" t="s">
+      <c r="A11" s="161" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="155" t="s">
+      <c r="A12" s="154" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="158" t="s">
         <v>508</v>
       </c>
-      <c r="B13" s="159">
+      <c r="B13" s="158">
         <v>84</v>
       </c>
-      <c r="C13" s="159" t="s">
+      <c r="C13" s="158" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="155" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="155" t="s">
+      <c r="A16" s="154" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="154" t="s">
+      <c r="A18" s="153" t="s">
         <v>513</v>
       </c>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="155" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="154" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="159" t="s">
+      <c r="A21" s="158" t="s">
         <v>515</v>
       </c>
-      <c r="B21" s="163">
+      <c r="B21" s="162">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="155" t="s">
+      <c r="A22" s="154" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="154" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="155" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="155" t="s">
         <v>518</v>
       </c>
     </row>

</xml_diff>